<commit_message>
ABC működik build done
</commit_message>
<xml_diff>
--- a/WindowsFormsApp autósiskola/bin/Debug/SablonFajl.xlsx
+++ b/WindowsFormsApp autósiskola/bin/Debug/SablonFajl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programozás\Extra projektek\WindowsFormsApp autósiskola\WindowsFormsApp autósiskola\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2958355-3203-413F-BEDC-948951CE81FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD65250-49AA-46A8-89CB-33E1A8EC73E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="1725" windowWidth="21600" windowHeight="11295" xr2:uid="{95E7278A-85B2-47E5-A576-31C77FD5FB75}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{95E7278A-85B2-47E5-A576-31C77FD5FB75}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
     <t>érdeklődött</t>
   </si>
   <si>
-    <t>E szerinti a sablon szerint állítsa be az oszlopok sorrendjét a programmal való működés miatt.(1 sor minta kitalált adatokkal) A sorszámozás mindenképpen az 'A2' cellától induljon növekvő sorrendben lefelé.  Az üres cellákba bármilyen adatot tárolhat, viszont mindeképpen legyen a "megjegyzések" az utolsó oszlop. A "felnőttképzési sz." és a "megjegyzések" oszlopok közé bármennyi plusz adat tehető. Mindig csináljon lehetőleg a biztonság kedvéért egy másik mentést az adott excel fájlról amit amit használ.</t>
+    <t>E szerinti a sablon szerint állítsa be az oszlopok sorrendjét a Főút autósiskola táblázattal való működés miatt.(1 sor minta kitalált adatokkal) A sorszámozás mindenképpen az 'A2' cellától induljon növekvő sorrendben lefelé.  Az üres cellákba bármilyen adatot tárolhat, viszont mindeképpen legyen a "megjegyzések" az utolsó oszlop. A "felnőttképzési sz." és a "megjegyzések" oszlopok közé bármennyi plusz adat tehető. Mindig csináljon lehetőleg a biztonság kedvéért egy másik mentést az adott excel fájlról amit amit használ.</t>
   </si>
 </sst>
 </file>

</xml_diff>